<commit_message>
created coins json file with all data for listing
</commit_message>
<xml_diff>
--- a/data/Top100Crypto.xlsx
+++ b/data/Top100Crypto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinyin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinyin/Desktop/React-Table/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="296">
   <si>
     <t>#</t>
   </si>
@@ -117,15 +117,6 @@
   </si>
   <si>
     <t>One Tether equals one USD — always.</t>
-  </si>
-  <si>
-    <t>IOTA</t>
-  </si>
-  <si>
-    <t>MIOTA</t>
-  </si>
-  <si>
-    <t>Blockchain meets the Internet-of-Things, with no transaction fees.</t>
   </si>
   <si>
     <t>Tron</t>
@@ -1263,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,7 +1404,7 @@
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -1427,7 +1418,7 @@
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>33</v>
@@ -1441,37 +1432,37 @@
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1483,9 +1474,9 @@
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1497,7 +1488,7 @@
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>47</v>
@@ -1511,7 +1502,7 @@
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>50</v>
@@ -1525,7 +1516,7 @@
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
@@ -1539,7 +1530,7 @@
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>56</v>
@@ -1553,7 +1544,7 @@
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>59</v>
@@ -1567,7 +1558,7 @@
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>62</v>
@@ -1581,7 +1572,7 @@
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -1595,7 +1586,7 @@
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>68</v>
@@ -1609,7 +1600,7 @@
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>71</v>
@@ -1623,7 +1614,7 @@
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>74</v>
@@ -1637,7 +1628,7 @@
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>77</v>
@@ -1645,13 +1636,13 @@
       <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>80</v>
@@ -1659,13 +1650,13 @@
       <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>83</v>
@@ -1679,9 +1670,9 @@
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1693,9 +1684,9 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1707,7 +1698,7 @@
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>92</v>
@@ -1721,7 +1712,7 @@
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>95</v>
@@ -1735,7 +1726,7 @@
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>98</v>
@@ -1743,13 +1734,13 @@
       <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>101</v>
@@ -1757,13 +1748,13 @@
       <c r="C35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>104</v>
@@ -1777,23 +1768,23 @@
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1805,7 +1796,7 @@
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>113</v>
@@ -1813,13 +1804,13 @@
       <c r="C39" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>116</v>
@@ -1833,7 +1824,7 @@
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>119</v>
@@ -1847,9 +1838,9 @@
     </row>
     <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -1861,9 +1852,9 @@
     </row>
     <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1875,7 +1866,7 @@
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>128</v>
@@ -1889,7 +1880,7 @@
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>131</v>
@@ -1903,7 +1894,7 @@
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>134</v>
@@ -1917,7 +1908,7 @@
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>137</v>
@@ -1931,7 +1922,7 @@
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>140</v>
@@ -1945,7 +1936,7 @@
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>143</v>
@@ -1959,21 +1950,21 @@
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>146</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>149</v>
@@ -1981,15 +1972,15 @@
       <c r="C51" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>51</v>
-      </c>
-      <c r="B52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>152</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -2001,9 +1992,9 @@
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -2015,7 +2006,7 @@
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>158</v>
@@ -2029,7 +2020,7 @@
     </row>
     <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>161</v>
@@ -2043,7 +2034,7 @@
     </row>
     <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>164</v>
@@ -2057,7 +2048,7 @@
     </row>
     <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>167</v>
@@ -2071,9 +2062,9 @@
     </row>
     <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>57</v>
-      </c>
-      <c r="B58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2085,9 +2076,9 @@
     </row>
     <row r="59" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2099,9 +2090,9 @@
     </row>
     <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>59</v>
-      </c>
-      <c r="B60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>176</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -2113,9 +2104,9 @@
     </row>
     <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -2127,7 +2118,7 @@
     </row>
     <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>182</v>
@@ -2141,9 +2132,9 @@
     </row>
     <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>62</v>
-      </c>
-      <c r="B63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>185</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2155,7 +2146,7 @@
     </row>
     <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>188</v>
@@ -2169,9 +2160,9 @@
     </row>
     <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>191</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2183,9 +2174,9 @@
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>65</v>
-      </c>
-      <c r="B66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>194</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2197,9 +2188,9 @@
     </row>
     <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2211,24 +2202,24 @@
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C68" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>68</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>203</v>
+        <v>69</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>203</v>
@@ -2239,9 +2230,9 @@
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>69</v>
-      </c>
-      <c r="B70" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>205</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -2253,7 +2244,7 @@
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>208</v>
@@ -2267,7 +2258,7 @@
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>211</v>
@@ -2281,7 +2272,7 @@
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>214</v>
@@ -2295,7 +2286,7 @@
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>217</v>
@@ -2309,7 +2300,7 @@
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>220</v>
@@ -2323,7 +2314,7 @@
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>223</v>
@@ -2337,7 +2328,7 @@
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>226</v>
@@ -2351,24 +2342,24 @@
     </row>
     <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>232</v>
@@ -2379,7 +2370,7 @@
     </row>
     <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>234</v>
@@ -2393,9 +2384,9 @@
     </row>
     <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>80</v>
-      </c>
-      <c r="B81" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -2407,9 +2398,9 @@
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>81</v>
-      </c>
-      <c r="B82" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -2421,7 +2412,7 @@
     </row>
     <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>243</v>
@@ -2435,7 +2426,7 @@
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>246</v>
@@ -2449,7 +2440,7 @@
     </row>
     <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>249</v>
@@ -2463,9 +2454,9 @@
     </row>
     <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>85</v>
-      </c>
-      <c r="B86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>252</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -2477,9 +2468,9 @@
     </row>
     <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>86</v>
-      </c>
-      <c r="B87" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>255</v>
       </c>
       <c r="C87" s="2" t="s">
@@ -2491,7 +2482,7 @@
     </row>
     <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>258</v>
@@ -2505,9 +2496,9 @@
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>88</v>
-      </c>
-      <c r="B89" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>261</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -2519,9 +2510,9 @@
     </row>
     <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>89</v>
-      </c>
-      <c r="B90" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>264</v>
       </c>
       <c r="C90" s="2" t="s">
@@ -2533,7 +2524,7 @@
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>267</v>
@@ -2547,7 +2538,7 @@
     </row>
     <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>270</v>
@@ -2561,7 +2552,7 @@
     </row>
     <row r="93" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>273</v>
@@ -2575,7 +2566,7 @@
     </row>
     <row r="94" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>276</v>
@@ -2589,7 +2580,7 @@
     </row>
     <row r="95" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>279</v>
@@ -2603,9 +2594,9 @@
     </row>
     <row r="96" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>95</v>
-      </c>
-      <c r="B96" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>282</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -2617,7 +2608,7 @@
     </row>
     <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>285</v>
@@ -2631,9 +2622,9 @@
     </row>
     <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>97</v>
-      </c>
-      <c r="B98" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>288</v>
       </c>
       <c r="C98" s="2" t="s">
@@ -2645,9 +2636,9 @@
     </row>
     <row r="99" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>98</v>
-      </c>
-      <c r="B99" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>291</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -2659,30 +2650,16 @@
     </row>
     <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A101" s="2">
-        <v>100</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2696,62 +2673,61 @@
     <hyperlink ref="B7" r:id="rId7" tooltip="Litecoin"/>
     <hyperlink ref="B8" r:id="rId8" tooltip="Stellar Lumens"/>
     <hyperlink ref="B9" r:id="rId9" tooltip="Cardano"/>
-    <hyperlink ref="B11" r:id="rId10" tooltip="IOTA"/>
-    <hyperlink ref="B12" r:id="rId11" tooltip="Tron"/>
-    <hyperlink ref="B13" r:id="rId12" tooltip="Monero"/>
-    <hyperlink ref="B14" r:id="rId13" tooltip="NEO"/>
-    <hyperlink ref="D14" r:id="rId14" tooltip="China’s Ethereum"/>
-    <hyperlink ref="B15" r:id="rId15" tooltip="Dash"/>
-    <hyperlink ref="B17" r:id="rId16" tooltip="Ethereum Classic"/>
-    <hyperlink ref="B18" r:id="rId17" tooltip="VeChain"/>
-    <hyperlink ref="B19" r:id="rId18" tooltip="NEM"/>
-    <hyperlink ref="B20" r:id="rId19" tooltip="Ontology"/>
-    <hyperlink ref="B21" r:id="rId20" tooltip="Qtum"/>
-    <hyperlink ref="B22" r:id="rId21" tooltip="OmiseGO"/>
-    <hyperlink ref="B23" r:id="rId22" tooltip="Zcash"/>
-    <hyperlink ref="B24" r:id="rId23" tooltip="ICON"/>
-    <hyperlink ref="B25" r:id="rId24" tooltip="Lisk"/>
-    <hyperlink ref="B26" r:id="rId25" tooltip="Decred"/>
-    <hyperlink ref="B27" r:id="rId26" tooltip="Zilliqa"/>
-    <hyperlink ref="B28" r:id="rId27" tooltip="Bytecoin"/>
-    <hyperlink ref="D28" r:id="rId28" tooltip="Privacy coin"/>
-    <hyperlink ref="B29" r:id="rId29" tooltip="Aeternity"/>
-    <hyperlink ref="B30" r:id="rId30" tooltip="Bitcoin Gold"/>
-    <hyperlink ref="B32" r:id="rId31" tooltip="Siacoin"/>
-    <hyperlink ref="B33" r:id="rId32" tooltip="BitShares"/>
-    <hyperlink ref="B34" r:id="rId33" tooltip="Verge"/>
-    <hyperlink ref="B35" r:id="rId34" tooltip="Steem"/>
-    <hyperlink ref="D35" r:id="rId35" tooltip="cryptocurrency payments"/>
-    <hyperlink ref="B36" r:id="rId36" tooltip="0x"/>
-    <hyperlink ref="B37" r:id="rId37" tooltip="Augur"/>
-    <hyperlink ref="D38" r:id="rId38" tooltip="suspicious"/>
-    <hyperlink ref="B39" r:id="rId39" tooltip="Maker"/>
-    <hyperlink ref="D39" r:id="rId40" tooltip="Stablecoin"/>
-    <hyperlink ref="B40" r:id="rId41" tooltip="Nano"/>
-    <hyperlink ref="B41" r:id="rId42" tooltip="Dogecoin"/>
-    <hyperlink ref="B42" r:id="rId43" tooltip="Waves"/>
-    <hyperlink ref="B44" r:id="rId44" tooltip="Golem"/>
-    <hyperlink ref="B45" r:id="rId45" tooltip="DigiByte"/>
-    <hyperlink ref="B46" r:id="rId46" tooltip="Nebulas"/>
-    <hyperlink ref="B47" r:id="rId47" tooltip="Stratis"/>
-    <hyperlink ref="B48" r:id="rId48" tooltip="Populous"/>
-    <hyperlink ref="B49" r:id="rId49" tooltip="Wanchain"/>
-    <hyperlink ref="B50" r:id="rId50" tooltip="Basic Attention Token"/>
-    <hyperlink ref="D51" r:id="rId51" tooltip="ZClassic"/>
-    <hyperlink ref="B53" r:id="rId52" tooltip="Status"/>
-    <hyperlink ref="B59" r:id="rId53" tooltip="Waltonchain"/>
-    <hyperlink ref="B61" r:id="rId54" tooltip="Aion"/>
-    <hyperlink ref="B64" r:id="rId55" tooltip="Bancor"/>
-    <hyperlink ref="B65" r:id="rId56" tooltip="MaidSafeCoin"/>
-    <hyperlink ref="B67" r:id="rId57" tooltip="Ardor"/>
-    <hyperlink ref="B70" r:id="rId58" tooltip="Ark"/>
-    <hyperlink ref="B82" r:id="rId59" tooltip="Elastos"/>
-    <hyperlink ref="B87" r:id="rId60" tooltip="Decentraland"/>
-    <hyperlink ref="B90" r:id="rId61" tooltip="Nxt"/>
-    <hyperlink ref="B97" r:id="rId62" tooltip="Scry.info"/>
-    <hyperlink ref="B98" r:id="rId63" tooltip="Factom"/>
-    <hyperlink ref="B100" r:id="rId64" tooltip="Nuls"/>
-    <hyperlink ref="B101" r:id="rId65" tooltip="QASH"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="Tron"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="Monero"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="NEO"/>
+    <hyperlink ref="D13" r:id="rId13" tooltip="China’s Ethereum"/>
+    <hyperlink ref="B14" r:id="rId14" tooltip="Dash"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="Ethereum Classic"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="VeChain"/>
+    <hyperlink ref="B18" r:id="rId17" tooltip="NEM"/>
+    <hyperlink ref="B19" r:id="rId18" tooltip="Ontology"/>
+    <hyperlink ref="B20" r:id="rId19" tooltip="Qtum"/>
+    <hyperlink ref="B21" r:id="rId20" tooltip="OmiseGO"/>
+    <hyperlink ref="B22" r:id="rId21" tooltip="Zcash"/>
+    <hyperlink ref="B23" r:id="rId22" tooltip="ICON"/>
+    <hyperlink ref="B24" r:id="rId23" tooltip="Lisk"/>
+    <hyperlink ref="B25" r:id="rId24" tooltip="Decred"/>
+    <hyperlink ref="B26" r:id="rId25" tooltip="Zilliqa"/>
+    <hyperlink ref="B27" r:id="rId26" tooltip="Bytecoin"/>
+    <hyperlink ref="D27" r:id="rId27" tooltip="Privacy coin"/>
+    <hyperlink ref="B28" r:id="rId28" tooltip="Aeternity"/>
+    <hyperlink ref="B29" r:id="rId29" tooltip="Bitcoin Gold"/>
+    <hyperlink ref="B31" r:id="rId30" tooltip="Siacoin"/>
+    <hyperlink ref="B32" r:id="rId31" tooltip="BitShares"/>
+    <hyperlink ref="B33" r:id="rId32" tooltip="Verge"/>
+    <hyperlink ref="B34" r:id="rId33" tooltip="Steem"/>
+    <hyperlink ref="D34" r:id="rId34" tooltip="cryptocurrency payments"/>
+    <hyperlink ref="B35" r:id="rId35" tooltip="0x"/>
+    <hyperlink ref="B36" r:id="rId36" tooltip="Augur"/>
+    <hyperlink ref="D37" r:id="rId37" tooltip="suspicious"/>
+    <hyperlink ref="B38" r:id="rId38" tooltip="Maker"/>
+    <hyperlink ref="D38" r:id="rId39" tooltip="Stablecoin"/>
+    <hyperlink ref="B39" r:id="rId40" tooltip="Nano"/>
+    <hyperlink ref="B40" r:id="rId41" tooltip="Dogecoin"/>
+    <hyperlink ref="B41" r:id="rId42" tooltip="Waves"/>
+    <hyperlink ref="B43" r:id="rId43" tooltip="Golem"/>
+    <hyperlink ref="B44" r:id="rId44" tooltip="DigiByte"/>
+    <hyperlink ref="B45" r:id="rId45" tooltip="Nebulas"/>
+    <hyperlink ref="B46" r:id="rId46" tooltip="Stratis"/>
+    <hyperlink ref="B47" r:id="rId47" tooltip="Populous"/>
+    <hyperlink ref="B48" r:id="rId48" tooltip="Wanchain"/>
+    <hyperlink ref="B49" r:id="rId49" tooltip="Basic Attention Token"/>
+    <hyperlink ref="D50" r:id="rId50" tooltip="ZClassic"/>
+    <hyperlink ref="B52" r:id="rId51" tooltip="Status"/>
+    <hyperlink ref="B58" r:id="rId52" tooltip="Waltonchain"/>
+    <hyperlink ref="B60" r:id="rId53" tooltip="Aion"/>
+    <hyperlink ref="B63" r:id="rId54" tooltip="Bancor"/>
+    <hyperlink ref="B64" r:id="rId55" tooltip="MaidSafeCoin"/>
+    <hyperlink ref="B66" r:id="rId56" tooltip="Ardor"/>
+    <hyperlink ref="B69" r:id="rId57" tooltip="Ark"/>
+    <hyperlink ref="B81" r:id="rId58" tooltip="Elastos"/>
+    <hyperlink ref="B86" r:id="rId59" tooltip="Decentraland"/>
+    <hyperlink ref="B89" r:id="rId60" tooltip="Nxt"/>
+    <hyperlink ref="B96" r:id="rId61" tooltip="Scry.info"/>
+    <hyperlink ref="B97" r:id="rId62" tooltip="Factom"/>
+    <hyperlink ref="B99" r:id="rId63" tooltip="Nuls"/>
+    <hyperlink ref="B100" r:id="rId64" tooltip="QASH"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>